<commit_message>
Módulo 10 - Gráficos dinâmicos parte 1
</commit_message>
<xml_diff>
--- a/módulo 10/aula-grafico-dinamico.xlsx
+++ b/módulo 10/aula-grafico-dinamico.xlsx
@@ -5,26 +5,80 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Documents\Curso Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BaseDeDados" sheetId="2" r:id="rId1"/>
+    <sheet name="TDVendas" sheetId="3" r:id="rId2"/>
+    <sheet name="Dashboard" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlcn.WorksheetConnection_aulagraficodinamico.xlsxTBVendas1" hidden="1">TBVendas[]</definedName>
+    <definedName name="SegmentaçãodeDados_Ano">#N/A</definedName>
+    <definedName name="SegmentaçãodeDados_Vendedor">#N/A</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="27" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
+      <x14:pivotCaches>
+        <pivotCache cacheId="21" r:id="rId5"/>
+      </x14:pivotCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{FCE2AD5D-F65C-4FA6-A056-5C36A1767C68}">
+      <x15:dataModel>
+        <x15:modelTables>
+          <x15:modelTable id="TBVendas-3e296435-892b-466d-bf80-c4983e9f5f61" name="TBVendas" connection="WorksheetConnection_aula-grafico-dinamico.xlsx!TBVendas"/>
+        </x15:modelTables>
+      </x15:dataModel>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="ThisWorkbookDataModel" description="Modelo de Dados" type="5" refreshedVersion="5" minRefreshableVersion="5" background="1">
+    <dbPr connection="Data Model Connection" command="Model" commandType="1"/>
+    <olapPr sendLocale="1" rowDrillCount="1000"/>
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="" model="1"/>
+      </ext>
+    </extLst>
+  </connection>
+  <connection id="2" name="WorksheetConnection_aula-grafico-dinamico.xlsx!TBVendas" type="102" refreshedVersion="5" minRefreshableVersion="5">
+    <extLst>
+      <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
+        <x15:connection id="TBVendas-3e296435-892b-466d-bf80-c4983e9f5f61" autoDelete="1">
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_aulagraficodinamico.xlsxTBVendas1"/>
+        </x15:connection>
+      </ext>
+    </extLst>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="21">
   <si>
     <t>Mês</t>
   </si>
@@ -67,17 +121,38 @@
   <si>
     <t>Negócios Fechados</t>
   </si>
+  <si>
+    <t>Rótulos de Linha</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>Rótulos de Coluna</t>
+  </si>
+  <si>
+    <t>Soma de Valor Vendido</t>
+  </si>
+  <si>
+    <t>Tirar os filtros do gráfico dinamico: clica no gráfico/analisar/Botões de campos/ocultar tudo</t>
+  </si>
+  <si>
+    <t>Painel de vendas</t>
+  </si>
+  <si>
+    <t>Inserir segmentação de dados: clica no gráfico/analisar/segmentação de dados</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +167,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -113,15 +216,15 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -129,6 +232,16 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -153,7 +266,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -190,7 +303,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -208,10 +321,10 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -236,6 +349,2203 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[aula-grafico-dinamico.xlsx]TDVendas!Tabela dinâmica1</c:name>
+    <c:fmtId val="2"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vendas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="16"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="17"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="18"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="19"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="20"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="21"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="22"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="23"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TDVendas!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Anakin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TDVendas!$A$5:$A$18</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2016</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TDVendas!$B$5:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>16020</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12624</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15883</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6436</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21707</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9788</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5681</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15541</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11731</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19349</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20795</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TDVendas!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Barry Allen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TDVendas!$A$5:$A$18</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2016</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TDVendas!$C$5:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>21591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21216</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14038</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10816</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7302</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12927</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15731</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21601</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19284</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11709</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10557</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12383</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1317400256"/>
+        <c:axId val="-1317412224"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1317400256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1317412224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1317412224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1317400256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371474</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>304801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Ano"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Ano"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="95250" y="876301"/>
+              <a:ext cx="1905000" cy="971550"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa uma segmentação de dados. Segmentações de dados têm suporte no Excel 2010 ou versões posteriores.
+\Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2003 ou versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Vendedor"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Vendedor"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="133350" y="1933576"/>
+              <a:ext cx="1885950" cy="1847850"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="pt-BR" sz="1100"/>
+                <a:t>Esta forma representa uma segmentação de dados. Segmentações de dados têm suporte no Excel 2010 ou versões posteriores.
+\Se a forma tiver sido modificada em uma versão anterior do Excel, ou se a pasta de trabalho tiver sido salva no Excel 2003 ou versões anteriores, a segmentação de dados não poderá ser usada.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Jai" refreshedDate="45369.626699768516" backgroundQuery="1" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="4">
+    <cacheField name="[TBVendas].[Ano].[Ano]" caption="Ano" numFmtId="0" hierarchy="1" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2016" maxValue="2016" count="1">
+        <n v="2016"/>
+      </sharedItems>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
+          <x15:cachedUniqueNames>
+            <x15:cachedUniqueName index="0" name="[TBVendas].[Ano].&amp;[2016]"/>
+          </x15:cachedUniqueNames>
+        </ext>
+      </extLst>
+    </cacheField>
+    <cacheField name="[TBVendas].[Mês].[Mês]" caption="Mês" numFmtId="0" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12" count="12">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
+        <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="8"/>
+        <n v="9"/>
+        <n v="10"/>
+        <n v="11"/>
+        <n v="12"/>
+      </sharedItems>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
+          <x15:cachedUniqueNames>
+            <x15:cachedUniqueName index="0" name="[TBVendas].[Mês].&amp;[1]"/>
+            <x15:cachedUniqueName index="1" name="[TBVendas].[Mês].&amp;[2]"/>
+            <x15:cachedUniqueName index="2" name="[TBVendas].[Mês].&amp;[3]"/>
+            <x15:cachedUniqueName index="3" name="[TBVendas].[Mês].&amp;[4]"/>
+            <x15:cachedUniqueName index="4" name="[TBVendas].[Mês].&amp;[5]"/>
+            <x15:cachedUniqueName index="5" name="[TBVendas].[Mês].&amp;[6]"/>
+            <x15:cachedUniqueName index="6" name="[TBVendas].[Mês].&amp;[7]"/>
+            <x15:cachedUniqueName index="7" name="[TBVendas].[Mês].&amp;[8]"/>
+            <x15:cachedUniqueName index="8" name="[TBVendas].[Mês].&amp;[9]"/>
+            <x15:cachedUniqueName index="9" name="[TBVendas].[Mês].&amp;[10]"/>
+            <x15:cachedUniqueName index="10" name="[TBVendas].[Mês].&amp;[11]"/>
+            <x15:cachedUniqueName index="11" name="[TBVendas].[Mês].&amp;[12]"/>
+          </x15:cachedUniqueNames>
+        </ext>
+      </extLst>
+    </cacheField>
+    <cacheField name="[TBVendas].[Vendedor].[Vendedor]" caption="Vendedor" numFmtId="0" hierarchy="2" level="1">
+      <sharedItems count="8">
+        <s v="Anakin"/>
+        <s v="Barry Allen"/>
+        <s v="Kal-El" u="1"/>
+        <s v="Logan" u="1"/>
+        <s v="Padmé Amidala" u="1"/>
+        <s v="Rachel Roth" u="1"/>
+        <s v="Victor Von Doom" u="1"/>
+        <s v="Wanda Maximoff" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Measures].[Soma de Valor Vendido]" caption="Soma de Valor Vendido" numFmtId="0" hierarchy="6" level="32767"/>
+  </cacheFields>
+  <cacheHierarchies count="9">
+    <cacheHierarchy uniqueName="[TBVendas].[Mês]" caption="Mês" attribute="1" defaultMemberUniqueName="[TBVendas].[Mês].[All]" allUniqueName="[TBVendas].[Mês].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[TBVendas].[Ano]" caption="Ano" attribute="1" defaultMemberUniqueName="[TBVendas].[Ano].[All]" allUniqueName="[TBVendas].[Ano].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[TBVendas].[Vendedor]" caption="Vendedor" attribute="1" defaultMemberUniqueName="[TBVendas].[Vendedor].[All]" allUniqueName="[TBVendas].[Vendedor].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[TBVendas].[Clientes visitados]" caption="Clientes visitados" attribute="1" defaultMemberUniqueName="[TBVendas].[Clientes visitados].[All]" allUniqueName="[TBVendas].[Clientes visitados].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Negócios Fechados]" caption="Negócios Fechados" attribute="1" defaultMemberUniqueName="[TBVendas].[Negócios Fechados].[All]" allUniqueName="[TBVendas].[Negócios Fechados].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Valor Vendido]" caption="Valor Vendido" attribute="1" defaultMemberUniqueName="[TBVendas].[Valor Vendido].[All]" allUniqueName="[TBVendas].[Valor Vendido].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Soma de Valor Vendido]" caption="Soma de Valor Vendido" measure="1" displayFolder="" measureGroup="TBVendas" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="3"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="5"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count TBVendas]" caption="__XL_Count TBVendas" measure="1" displayFolder="" measureGroup="TBVendas" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count of Models]" caption="__XL_Count of Models" measure="1" displayFolder="" count="0" hidden="1"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="TBVendas" uniqueName="[TBVendas]" caption="TBVendas"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="TBVendas" caption="TBVendas"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Jai" refreshedDate="45369.626318865739" backgroundQuery="1" createdVersion="3" refreshedVersion="5" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="1">
+    <extLst>
+      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
+        <x14:sourceConnection name="ThisWorkbookDataModel"/>
+      </ext>
+    </extLst>
+  </cacheSource>
+  <cacheFields count="0"/>
+  <cacheHierarchies count="9">
+    <cacheHierarchy uniqueName="[TBVendas].[Mês]" caption="Mês" attribute="1" defaultMemberUniqueName="[TBVendas].[Mês].[All]" allUniqueName="[TBVendas].[Mês].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Ano]" caption="Ano" attribute="1" defaultMemberUniqueName="[TBVendas].[Ano].[All]" allUniqueName="[TBVendas].[Ano].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Vendedor]" caption="Vendedor" attribute="1" defaultMemberUniqueName="[TBVendas].[Vendedor].[All]" allUniqueName="[TBVendas].[Vendedor].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="2" memberValueDatatype="130" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Clientes visitados]" caption="Clientes visitados" attribute="1" defaultMemberUniqueName="[TBVendas].[Clientes visitados].[All]" allUniqueName="[TBVendas].[Clientes visitados].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Negócios Fechados]" caption="Negócios Fechados" attribute="1" defaultMemberUniqueName="[TBVendas].[Negócios Fechados].[All]" allUniqueName="[TBVendas].[Negócios Fechados].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[TBVendas].[Valor Vendido]" caption="Valor Vendido" attribute="1" defaultMemberUniqueName="[TBVendas].[Valor Vendido].[All]" allUniqueName="[TBVendas].[Valor Vendido].[All]" dimensionUniqueName="[TBVendas]" displayFolder="" count="0" memberValueDatatype="20" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Soma de Valor Vendido]" caption="Soma de Valor Vendido" measure="1" displayFolder="" measureGroup="TBVendas" count="0">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="5"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count TBVendas]" caption="__XL_Count TBVendas" measure="1" displayFolder="" measureGroup="TBVendas" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count of Models]" caption="__XL_Count of Models" measure="1" displayFolder="" count="0" hidden="1"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition slicerData="1" pivotCacheId="1" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="A3:D18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="2">
+        <item s="1" x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="9">
+        <item s="1" x="0"/>
+        <item s="1" x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="14">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Soma de Valor Vendido" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="16">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="16" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="17" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="18" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="20" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="21" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="23" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotHierarchies count="9">
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+  </pivotHierarchies>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <rowHierarchiesUsage count="2">
+    <rowHierarchyUsage hierarchyUsage="1"/>
+    <rowHierarchyUsage hierarchyUsage="0"/>
+  </rowHierarchiesUsage>
+  <colHierarchiesUsage count="1">
+    <colHierarchyUsage hierarchyUsage="2"/>
+  </colHierarchiesUsage>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{E67621CE-5B39-4880-91FE-76760E9C1902}">
+      <x15:pivotTableUISettings sourceDataName="WorksheetConnection_aula-grafico-dinamico.xlsx!TBVendas">
+        <x15:activeTabTopLevelEntity name="[TBVendas]"/>
+      </x15:pivotTableUISettings>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Ano" sourceName="[TBVendas].[Ano]">
+  <pivotTables>
+    <pivotTable tabId="3" name="Tabela dinâmica1"/>
+  </pivotTables>
+  <data>
+    <olap pivotCacheId="1">
+      <levels count="2">
+        <level uniqueName="[TBVendas].[Ano].[(All)]" sourceCaption="(All)" count="0"/>
+        <level uniqueName="[TBVendas].[Ano].[Ano]" sourceCaption="Ano" count="3">
+          <ranges>
+            <range startItem="0">
+              <i n="[TBVendas].[Ano].&amp;[2016]" c="2016"/>
+              <i n="[TBVendas].[Ano].&amp;[2017]" c="2017"/>
+              <i n="[TBVendas].[Ano].&amp;[2018]" c="2018"/>
+            </range>
+          </ranges>
+        </level>
+      </levels>
+      <selections count="1">
+        <selection n="[TBVendas].[Ano].&amp;[2016]"/>
+      </selections>
+    </olap>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="SegmentaçãodeDados_Vendedor" sourceName="[TBVendas].[Vendedor]">
+  <pivotTables>
+    <pivotTable tabId="3" name="Tabela dinâmica1"/>
+  </pivotTables>
+  <data>
+    <olap pivotCacheId="1">
+      <levels count="2">
+        <level uniqueName="[TBVendas].[Vendedor].[(All)]" sourceCaption="(All)" count="0"/>
+        <level uniqueName="[TBVendas].[Vendedor].[Vendedor]" sourceCaption="Vendedor" count="8">
+          <ranges>
+            <range startItem="0">
+              <i n="[TBVendas].[Vendedor].&amp;[Anakin]" c="Anakin"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Barry Allen]" c="Barry Allen"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Kal-El]" c="Kal-El"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Logan]" c="Logan"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Padmé Amidala]" c="Padmé Amidala"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Rachel Roth]" c="Rachel Roth"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Victor Von Doom]" c="Victor Von Doom"/>
+              <i n="[TBVendas].[Vendedor].&amp;[Wanda Maximoff]" c="Wanda Maximoff"/>
+            </range>
+          </ranges>
+        </level>
+      </levels>
+      <selections count="2">
+        <selection n="[TBVendas].[Vendedor].&amp;[Anakin]"/>
+        <selection n="[TBVendas].[Vendedor].&amp;[Barry Allen]"/>
+      </selections>
+    </olap>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <slicer name="Ano" cache="SegmentaçãodeDados_Ano" caption="Ano" columnCount="3" level="1" style="SlicerStyleLight6" rowHeight="241300"/>
+  <slicer name="Vendedor" cache="SegmentaçãodeDados_Vendedor" caption="Vendedor" level="1" style="SlicerStyleLight6" rowHeight="241300"/>
+</slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,7 +2862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6029,4 +8341,315 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="B5" s="8">
+        <v>176775</v>
+      </c>
+      <c r="C5" s="8">
+        <v>179155</v>
+      </c>
+      <c r="D5" s="8">
+        <v>355930</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8">
+        <v>16020</v>
+      </c>
+      <c r="C6" s="8">
+        <v>21591</v>
+      </c>
+      <c r="D6" s="8">
+        <v>37611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8">
+        <v>12624</v>
+      </c>
+      <c r="C7" s="8">
+        <v>21216</v>
+      </c>
+      <c r="D7" s="8">
+        <v>33840</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8">
+        <v>15883</v>
+      </c>
+      <c r="C8" s="8">
+        <v>14038</v>
+      </c>
+      <c r="D8" s="8">
+        <v>29921</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8">
+        <v>6436</v>
+      </c>
+      <c r="C9" s="8">
+        <v>10816</v>
+      </c>
+      <c r="D9" s="8">
+        <v>17252</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="8">
+        <v>21220</v>
+      </c>
+      <c r="C10" s="8">
+        <v>7302</v>
+      </c>
+      <c r="D10" s="8">
+        <v>28522</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="8">
+        <v>21707</v>
+      </c>
+      <c r="C11" s="8">
+        <v>12927</v>
+      </c>
+      <c r="D11" s="8">
+        <v>34634</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>7</v>
+      </c>
+      <c r="B12" s="8">
+        <v>9788</v>
+      </c>
+      <c r="C12" s="8">
+        <v>15731</v>
+      </c>
+      <c r="D12" s="8">
+        <v>25519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>8</v>
+      </c>
+      <c r="B13" s="8">
+        <v>5681</v>
+      </c>
+      <c r="C13" s="8">
+        <v>21601</v>
+      </c>
+      <c r="D13" s="8">
+        <v>27282</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>9</v>
+      </c>
+      <c r="B14" s="8">
+        <v>15541</v>
+      </c>
+      <c r="C14" s="8">
+        <v>19284</v>
+      </c>
+      <c r="D14" s="8">
+        <v>34825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>10</v>
+      </c>
+      <c r="B15" s="8">
+        <v>11731</v>
+      </c>
+      <c r="C15" s="8">
+        <v>11709</v>
+      </c>
+      <c r="D15" s="8">
+        <v>23440</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>11</v>
+      </c>
+      <c r="B16" s="8">
+        <v>19349</v>
+      </c>
+      <c r="C16" s="8">
+        <v>10557</v>
+      </c>
+      <c r="D16" s="8">
+        <v>29906</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>12</v>
+      </c>
+      <c r="B17" s="8">
+        <v>20795</v>
+      </c>
+      <c r="C17" s="8">
+        <v>12383</v>
+      </c>
+      <c r="D17" s="8">
+        <v>33178</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="8">
+        <v>176775</v>
+      </c>
+      <c r="C18" s="8">
+        <v>179155</v>
+      </c>
+      <c r="D18" s="8">
+        <v>355930</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.140625" customWidth="1"/>
+    <col min="21" max="21" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+    </row>
+    <row r="2" spans="1:21" ht="85.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>